<commit_message>
AFDP-2536: make FOIA case file rules safe when queue has not been set
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-foia.xlsx
+++ b/acm/rules/drools-case-file-rules-foia.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\foia-extension\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmiller\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16390" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,31 +187,31 @@
     <t>Nullify Billing Enter Date</t>
   </si>
   <si>
-    <t>queue.name != 'Billing'</t>
-  </si>
-  <si>
     <t>setBillingEnterDate, null</t>
   </si>
   <si>
-    <t>queue.name == 'Hold' &amp;&amp; holdEnterDate == null</t>
-  </si>
-  <si>
     <t>setHoldEnterDate, java.time.LocalDate.now()</t>
   </si>
   <si>
-    <t>queue.name == 'Billing' &amp;&amp; billingEnterDate == null</t>
-  </si>
-  <si>
     <t>Set Hold Enter Date</t>
   </si>
   <si>
     <t>Nullify Hold Enter Date</t>
   </si>
   <si>
-    <t>queue.name != 'Hold'</t>
-  </si>
-  <si>
     <t>setHoldEnterDate, null</t>
+  </si>
+  <si>
+    <t>queue?.name == 'Billing' &amp;&amp; billingEnterDate == null</t>
+  </si>
+  <si>
+    <t>queue?.name == 'Hold' &amp;&amp; holdEnterDate == null</t>
+  </si>
+  <si>
+    <t>queue?.name != 'Hold' &amp;&amp; holdEnterDate != null</t>
+  </si>
+  <si>
+    <t>queue?.name != 'Billing' &amp;&amp; billingEnterDate != null</t>
   </si>
 </sst>
 </file>
@@ -885,20 +885,19 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.3984375"/>
-    <col min="2" max="2" width="24.265625"/>
-    <col min="3" max="3" width="50.1328125"/>
-    <col min="4" max="4" width="100.3984375"/>
-    <col min="5" max="5" width="27.73046875"/>
-    <col min="6" max="1025" width="8.73046875"/>
+    <col min="1" max="1" width="19.36328125"/>
+    <col min="2" max="2" width="24.26953125"/>
+    <col min="3" max="3" width="50.08984375"/>
+    <col min="4" max="4" width="100.36328125"/>
+    <col min="5" max="5" width="27.7265625"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -908,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -918,7 +917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -928,7 +927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -938,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -948,7 +947,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -958,7 +957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -968,7 +967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -978,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -988,7 +987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -998,7 +997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1008,7 +1007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1018,7 +1017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="319" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1028,7 +1027,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1038,7 +1037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -1046,7 +1045,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1056,7 +1055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1064,7 +1063,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1074,7 +1073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>25</v>
@@ -1100,7 +1099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>28</v>
@@ -1112,7 +1111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>31</v>
@@ -1124,7 +1123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>34</v>
@@ -1136,7 +1135,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>37</v>
@@ -1148,7 +1147,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>40</v>
@@ -1160,61 +1159,61 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
     </row>
   </sheetData>
@@ -1229,10 +1228,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1025" width="8.73046875"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1245,10 +1241,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1025" width="8.73046875"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
AFDP-2522: Update of foia drools rule files
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-foia.xlsx
+++ b/acm/rules/drools-case-file-rules-foia.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmiller\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\foia-extension\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16390" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,31 +187,31 @@
     <t>Nullify Billing Enter Date</t>
   </si>
   <si>
+    <t>queue.name != 'Billing'</t>
+  </si>
+  <si>
     <t>setBillingEnterDate, null</t>
   </si>
   <si>
+    <t>queue.name == 'Hold' &amp;&amp; holdEnterDate == null</t>
+  </si>
+  <si>
     <t>setHoldEnterDate, java.time.LocalDate.now()</t>
   </si>
   <si>
+    <t>queue.name == 'Billing' &amp;&amp; billingEnterDate == null</t>
+  </si>
+  <si>
     <t>Set Hold Enter Date</t>
   </si>
   <si>
     <t>Nullify Hold Enter Date</t>
   </si>
   <si>
+    <t>queue.name != 'Hold'</t>
+  </si>
+  <si>
     <t>setHoldEnterDate, null</t>
-  </si>
-  <si>
-    <t>queue?.name == 'Billing' &amp;&amp; billingEnterDate == null</t>
-  </si>
-  <si>
-    <t>queue?.name == 'Hold' &amp;&amp; holdEnterDate == null</t>
-  </si>
-  <si>
-    <t>queue?.name != 'Hold' &amp;&amp; holdEnterDate != null</t>
-  </si>
-  <si>
-    <t>queue?.name != 'Billing' &amp;&amp; billingEnterDate != null</t>
   </si>
 </sst>
 </file>
@@ -885,19 +885,20 @@
   <dimension ref="A2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.36328125"/>
-    <col min="2" max="2" width="24.26953125"/>
-    <col min="3" max="3" width="50.08984375"/>
-    <col min="4" max="4" width="100.36328125"/>
-    <col min="5" max="5" width="27.7265625"/>
+    <col min="1" max="1" width="19.3984375"/>
+    <col min="2" max="2" width="24.265625"/>
+    <col min="3" max="3" width="50.1328125"/>
+    <col min="4" max="4" width="100.3984375"/>
+    <col min="5" max="5" width="27.73046875"/>
+    <col min="6" max="1025" width="8.73046875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -907,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -917,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -927,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -937,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -947,7 +948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -957,7 +958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -967,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -977,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -987,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -997,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1007,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1017,7 +1018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="319" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1027,7 +1028,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1037,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -1045,7 +1046,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1055,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1063,7 +1064,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1073,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>25</v>
@@ -1099,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>28</v>
@@ -1111,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>31</v>
@@ -1123,7 +1124,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>34</v>
@@ -1135,7 +1136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>37</v>
@@ -1147,7 +1148,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>40</v>
@@ -1159,61 +1160,61 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>55</v>
-      </c>
       <c r="D30" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>56</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
     </row>
   </sheetData>
@@ -1228,7 +1229,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1025" width="8.73046875"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1241,7 +1245,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1025" width="8.73046875"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
AFDP-2522 ensure case files rules work before queue has been assigned
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-foia.xlsx
+++ b/acm/rules/drools-case-file-rules-foia.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\foia-extension\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmiller.ARMEDIA\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" tabRatio="111"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -187,31 +187,31 @@
     <t>Nullify Billing Enter Date</t>
   </si>
   <si>
-    <t>queue.name != 'Billing'</t>
-  </si>
-  <si>
     <t>setBillingEnterDate, null</t>
   </si>
   <si>
-    <t>queue.name == 'Hold' &amp;&amp; holdEnterDate == null</t>
-  </si>
-  <si>
     <t>setHoldEnterDate, java.time.LocalDate.now()</t>
   </si>
   <si>
-    <t>queue.name == 'Billing' &amp;&amp; billingEnterDate == null</t>
-  </si>
-  <si>
     <t>Set Hold Enter Date</t>
   </si>
   <si>
     <t>Nullify Hold Enter Date</t>
   </si>
   <si>
-    <t>queue.name != 'Hold'</t>
-  </si>
-  <si>
     <t>setHoldEnterDate, null</t>
+  </si>
+  <si>
+    <t>queue?.name == 'Billing' &amp;&amp; billingEnterDate == null</t>
+  </si>
+  <si>
+    <t>queue?.name != 'Billing'</t>
+  </si>
+  <si>
+    <t>queue?.name == 'Hold' &amp;&amp; holdEnterDate == null</t>
+  </si>
+  <si>
+    <t>queue?.name != 'Hold'</t>
   </si>
 </sst>
 </file>
@@ -882,23 +882,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D33"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375"/>
-    <col min="2" max="2" width="24.265625"/>
-    <col min="3" max="3" width="50.1328125"/>
-    <col min="4" max="4" width="100.3984375"/>
-    <col min="5" max="5" width="27.73046875"/>
-    <col min="6" max="1025" width="8.73046875"/>
+    <col min="1" max="1" width="19.375"/>
+    <col min="2" max="2" width="24.25"/>
+    <col min="3" max="3" width="50.125"/>
+    <col min="4" max="4" width="100.375"/>
+    <col min="5" max="5" width="27.75"/>
+    <col min="6" max="1025" width="8.75"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -918,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -928,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -948,7 +948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -958,7 +958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -968,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -978,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -988,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -998,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1008,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1018,7 +1018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -1028,7 +1028,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1038,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1056,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1074,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>25</v>
@@ -1100,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>28</v>
@@ -1112,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>31</v>
@@ -1124,7 +1124,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>34</v>
@@ -1136,7 +1136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>37</v>
@@ -1148,7 +1148,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
         <v>40</v>
@@ -1160,62 +1160,56 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1229,9 +1223,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1245,9 +1239,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-2255 Changed configiration to set the due date to 30 days ahead of creation date.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-case-file-rules-foia.xlsx
+++ b/acm/rules/drools-case-file-rules-foia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmiller.ARMEDIA\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>dueDate == null</t>
-  </si>
-  <si>
-    <t>setDueDate, addDays(180)</t>
   </si>
   <si>
     <t>Set Received Date</t>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>queue?.name != 'Hold'</t>
+  </si>
+  <si>
+    <t>setDueDate, addDays(30)</t>
   </si>
 </sst>
 </file>
@@ -885,20 +885,20 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.375"/>
-    <col min="2" max="2" width="24.25"/>
-    <col min="3" max="3" width="50.125"/>
-    <col min="4" max="4" width="100.375"/>
-    <col min="5" max="5" width="27.75"/>
-    <col min="6" max="1025" width="8.75"/>
+    <col min="1" max="1" width="19.3984375"/>
+    <col min="2" max="2" width="24.265625"/>
+    <col min="3" max="3" width="50.1328125"/>
+    <col min="4" max="4" width="100.3984375"/>
+    <col min="5" max="5" width="27.73046875"/>
+    <col min="6" max="1025" width="8.73046875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -908,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -918,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -928,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -938,17 +938,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -958,7 +958,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -968,7 +968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -978,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -988,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -998,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -1008,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -1018,17 +1018,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="330" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -1038,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -1056,15 +1056,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -1074,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>25</v>
@@ -1100,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>28</v>
@@ -1112,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>31</v>
@@ -1124,7 +1124,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>34</v>
@@ -1136,7 +1136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>37</v>
@@ -1145,70 +1145,70 @@
         <v>38</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>41</v>
-      </c>
       <c r="D27" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
     </row>
   </sheetData>
@@ -1223,9 +1223,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.73046875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1239,9 +1239,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.73046875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>